<commit_message>
adding a bodge for making everything work with the eclipse site instead of the the new borealis site
</commit_message>
<xml_diff>
--- a/predicted outputs/predictedOutput1.xlsx
+++ b/predicted outputs/predictedOutput1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sdsmt0-my.sharepoint.com/personal/mathew_clutter_mines_sdsmt_edu/Documents/BOREALIS/Ground_Station_Tracker_GUI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sdsmt0-my.sharepoint.com/personal/mathew_clutter_mines_sdsmt_edu/Documents/BOREALIS/Ground_Station_Tracker_GUI/predicted outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{9001A72C-9950-4049-A73A-06207FA0919F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:40009_{9001A72C-9950-4049-A73A-06207FA0919F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90667DA8-474A-4D6A-9E85-AEC993040B46}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25320" yWindow="-4170" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="predictedOutput" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="13">
   <si>
     <t>Distance</t>
   </si>
@@ -58,7 +58,19 @@
     <t>server azimuth</t>
   </si>
   <si>
-    <t>server elevatoin</t>
+    <t>server elevation</t>
+  </si>
+  <si>
+    <t>Azimuth change without prediction</t>
+  </si>
+  <si>
+    <t>Average Azimuth change without prediction</t>
+  </si>
+  <si>
+    <t>Azimuth change with prediction</t>
+  </si>
+  <si>
+    <t>Average Azimuth change with prediciton</t>
   </si>
 </sst>
 </file>
@@ -542,8 +554,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -6652,7 +6670,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>server elevatoin</c:v>
+                  <c:v>server elevation</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -12046,10 +12064,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H434"/>
+  <dimension ref="A1:N434"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12058,32 +12076,48 @@
     <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" customWidth="1"/>
+    <col min="14" max="14" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:14" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>172.51890331143801</v>
       </c>
@@ -12108,8 +12142,24 @@
         <f>IF(D2="r",C2,0)</f>
         <v>40.787390162786998</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <f>ABS(G164-G2)</f>
+        <v>37.947544853697025</v>
+      </c>
+      <c r="K2">
+        <f>AVERAGE(J:J)</f>
+        <v>8.7287991294886371</v>
+      </c>
+      <c r="M2">
+        <f>ABS(B164-B162)</f>
+        <v>34.648114829380006</v>
+      </c>
+      <c r="N2">
+        <f>AVERAGE(M:M)</f>
+        <v>5.2440309109110919</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F3">
         <f t="shared" ref="F3:F66" si="0">IF(D3="r",A3,0)</f>
         <v>0</v>
@@ -12122,8 +12172,16 @@
         <f t="shared" ref="H3:H66" si="2">IF(D3="r",C3,0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <f>ABS(G178-G164)</f>
+        <v>0.91558270991600921</v>
+      </c>
+      <c r="M3">
+        <f>ABS(B178-B176)</f>
+        <v>1.6451718357899949</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>172.58078418994501</v>
       </c>
@@ -12148,8 +12206,16 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <f>ABS(G200-G178)</f>
+        <v>0.46448932781598273</v>
+      </c>
+      <c r="M4">
+        <f>ABS(B200-B198)</f>
+        <v>0.42541426167599639</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F5">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -12162,8 +12228,16 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <f>ABS(G220-G200)</f>
+        <v>2.1940540424640176</v>
+      </c>
+      <c r="M5">
+        <f>ABS(B220-B218)</f>
+        <v>1.3316018997120125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>172.64273535380201</v>
       </c>
@@ -12188,8 +12262,16 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <f>ABS(G240-G220)</f>
+        <v>3.2349068574930016</v>
+      </c>
+      <c r="M6">
+        <f>ABS(B240-B238)</f>
+        <v>5.3656877521669912</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F7">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -12202,8 +12284,16 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <f>ABS(G262-G240)</f>
+        <v>8.1961345772839991</v>
+      </c>
+      <c r="M7">
+        <f>ABS(B262-B260)</f>
+        <v>3.9364681204280032</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>172.704756730578</v>
       </c>
@@ -12228,8 +12318,16 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <f>ABS(G282-G262)</f>
+        <v>11.929407889687013</v>
+      </c>
+      <c r="M8">
+        <f>ABS(B282-B280)</f>
+        <v>3.0610796035600174</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -12242,8 +12340,16 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <f>ABS(G302-G282)</f>
+        <v>12.349900296495008</v>
+      </c>
+      <c r="M9">
+        <f>ABS(B302-B300)</f>
+        <v>1.392745351328017</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>172.766848243174</v>
       </c>
@@ -12268,8 +12374,16 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <f>ABS(G316-G302)</f>
+        <v>10.058375952262963</v>
+      </c>
+      <c r="M10">
+        <f>ABS(B316-B314)</f>
+        <v>2.9478228416109573</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F11">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -12282,8 +12396,16 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <f>ABS(G324-G316)</f>
+        <v>4.5543311330720258</v>
+      </c>
+      <c r="M11">
+        <f>ABS(B324-B322)</f>
+        <v>1.7661740244290058</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>172.82900981736401</v>
       </c>
@@ -12308,8 +12430,16 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <f>ABS(G342-G324)</f>
+        <v>4.1720627841879718</v>
+      </c>
+      <c r="M12">
+        <f>ABS(B342-B340)</f>
+        <v>1.1640594999410041</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -12323,7 +12453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>172.891241375964</v>
       </c>
@@ -12349,7 +12479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F15">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -12363,7 +12493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>172.95354284393201</v>
       </c>
@@ -20758,7 +20888,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>

</xml_diff>